<commit_message>
Update to support full month names and Resources column format. Add simplified Excel-only generator.
</commit_message>
<xml_diff>
--- a/sample_tasks.xlsx
+++ b/sample_tasks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Task1</t>
+          <t>Task 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -451,82 +451,77 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Resource</t>
+          <t>Resources</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Group</t>
+          <t>Data</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Data</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>January</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>February</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Feb</t>
+          <t>March</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Mar</t>
+          <t>April</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Apr</t>
+          <t>May</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>June</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Jun</t>
+          <t>July</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Jul</t>
+          <t>August</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Aug</t>
+          <t>September</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Sep</t>
+          <t>October</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Oct</t>
+          <t>November</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Dec</t>
+          <t>December</t>
         </is>
       </c>
     </row>
@@ -553,17 +548,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>New York</t>
+          <t>X</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -571,11 +566,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -585,7 +576,6 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -610,30 +600,26 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Analysis</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t>New York</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -642,7 +628,6 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -667,31 +652,27 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>San Francisco</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -699,7 +680,6 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -724,22 +704,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
           <t>San Francisco</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>X</t>
@@ -750,17 +730,12 @@
           <t>X</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -785,24 +760,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
           <t>Bangalore</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>X</t>
@@ -813,15 +788,10 @@
           <t>X</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -846,39 +816,34 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
           <t>New York</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="O7" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -903,19 +868,15 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Operations</t>
+          <t>High</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
           <t>London</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
@@ -924,14 +885,13 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -956,19 +916,15 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Training</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
           <t>London</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
@@ -977,18 +933,17 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="Q9" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1013,19 +968,15 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Documentation</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
           <t>Bangalore</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -1033,7 +984,11 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="P10" t="inlineStr">
         <is>
           <t>X</t>
@@ -1044,12 +999,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1074,19 +1024,15 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Management</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
           <t>New York</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -1097,8 +1043,7 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>X</t>
         </is>

</xml_diff>